<commit_message>
some html and css
</commit_message>
<xml_diff>
--- a/Tracker Update.xlsx
+++ b/Tracker Update.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
   <si>
     <t>DATE</t>
   </si>
@@ -387,7 +387,7 @@
     <t xml:space="preserve">JS Additional Topics through js course</t>
   </si>
   <si>
-    <t xml:space="preserve">Array, Function, Variables, Control Structure, Conditional Statement, Looping Statement, Js Functions, Js Scropes &amp; Closures, Arrow Function</t>
+    <t xml:space="preserve">Array, Function, Variables, Control Structure, Conditional Statement, Looping Statement, Js Functions, Js Scopes &amp; Closures, Arrow Function</t>
   </si>
   <si>
     <r>
@@ -782,6 +782,15 @@
 Jquery Get - text,html,val
 Jquery Set - text,html,val
 </t>
+  </si>
+  <si>
+    <t>Feathers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initialize Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create feathers app, Generate feather's service, Assign sevice route, implement mongodb connection, generate authentication, create schema file based on mongodb, Generate app</t>
   </si>
 </sst>
 </file>
@@ -887,7 +896,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -946,7 +955,13 @@
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1459,7 +1474,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C5" zoomScale="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A26" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1975,8 +1990,20 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" ht="14.25">
-      <c r="E28" s="20"/>
+    <row r="28" ht="57">
+      <c r="A28" s="20">
+        <v>46358</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28" s="22"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="1"/>

</xml_diff>